<commit_message>
Start ignoring db and xlsx files
</commit_message>
<xml_diff>
--- a/inventory/spreadsheet_backups/inventory_data.xlsx
+++ b/inventory/spreadsheet_backups/inventory_data.xlsx
@@ -71288,7 +71288,7 @@
         <v>inventoryadmin</v>
       </c>
       <c r="D2" t="str">
-        <v>$2b$10$.N/HGn3fLy2vWrwd15D/d.Eh0q8a.4eGsv8IJz5oV/.5Seo7J1a3W</v>
+        <v>$2b$10$Ryh0dEgzRo334kYjyqZQq.MpN9v5ziDq7w1U9bSfp5rNAjMfqnr/.</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -71297,10 +71297,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="str">
-        <v>$2b$10$.N/HGn3fLy2vWrwd15D/d.</v>
+        <v>$2b$10$Ryh0dEgzRo334kYjyqZQq.</v>
       </c>
       <c r="H2" t="str">
-        <v>2022-12-12 18:12:43</v>
+        <v>2022-12-14 23:11:46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>